<commit_message>
Print xlsx halaman menu Data Invoice
</commit_message>
<xml_diff>
--- a/liquiditas-monitoring/src/main/resources/templates/report/template_rekap_all_invoice.xlsx
+++ b/liquiditas-monitoring/src/main/resources/templates/report/template_rekap_all_invoice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6469134A-3FE5-487E-8D7F-C2244305F765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2D3AD2-6141-46ED-9AC9-899950D74F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="2670" windowWidth="23715" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21540" yWindow="2085" windowWidth="25020" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>${TITLE}</t>
   </si>
@@ -49,48 +49,9 @@
     <t>${detail.ROW_NUMBER}</t>
   </si>
   <si>
-    <t>DOCUMENT NUMBER</t>
-  </si>
-  <si>
-    <t>DOCUMENT TYPE</t>
-  </si>
-  <si>
-    <t>COMPANY CODE</t>
-  </si>
-  <si>
-    <t>FISCAL YEAR</t>
-  </si>
-  <si>
-    <t>BUSINESS AREA</t>
-  </si>
-  <si>
-    <t>DOCUMENT DATE</t>
-  </si>
-  <si>
-    <t>POST DATE</t>
-  </si>
-  <si>
-    <t>ENTRY DATE</t>
-  </si>
-  <si>
-    <t>DOCUMENT HDR TEXT</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
     <t>EXCHANGE RATE</t>
   </si>
   <si>
-    <t>TRANSACTION TYPE</t>
-  </si>
-  <si>
-    <t>OSS ID</t>
-  </si>
-  <si>
-    <t>SUMBER DANA</t>
-  </si>
-  <si>
     <t>TGL RENCANA BAYAR</t>
   </si>
   <si>
@@ -100,181 +61,70 @@
     <t>CURRENCY BAYAR</t>
   </si>
   <si>
-    <t>BANK BENEFICIARY</t>
-  </si>
-  <si>
-    <t>NAMA BENEFICIARY</t>
-  </si>
-  <si>
-    <t>JENIS BAYAR</t>
-  </si>
-  <si>
-    <t>JENIS DOKUMEN</t>
-  </si>
-  <si>
-    <t>NAMA UNIT</t>
-  </si>
-  <si>
-    <t>TGL TERIMA TAGIHAN</t>
-  </si>
-  <si>
-    <t>INPUT BY</t>
-  </si>
-  <si>
-    <t>LINE NUMBER</t>
-  </si>
-  <si>
-    <t>AMOUNT LC</t>
-  </si>
-  <si>
-    <t>AMOUNT TC</t>
-  </si>
-  <si>
-    <t>AMOUNT WITH BASE LC</t>
-  </si>
-  <si>
-    <t>AMOUNT WITH LC</t>
-  </si>
-  <si>
-    <t>AMOUNT WITH BASE TC</t>
-  </si>
-  <si>
-    <t>AMOUNT WITH TC</t>
-  </si>
-  <si>
-    <t>TOTAL AMOUNT TC</t>
-  </si>
-  <si>
-    <t>TOTAL AMOUNT LC</t>
-  </si>
-  <si>
-    <t>ASSIGMENT</t>
-  </si>
-  <si>
-    <t>ITEM TEXT</t>
-  </si>
-  <si>
-    <t>CUSTOMER</t>
-  </si>
-  <si>
-    <t>CUSTOMER NAME</t>
-  </si>
-  <si>
-    <t>VENDOR NAME</t>
-  </si>
-  <si>
-    <t>${detail.DOC_NO}</t>
-  </si>
-  <si>
-    <t>${detail.DOC_TYPE}</t>
-  </si>
-  <si>
-    <t>${detail.COMP_CODE}</t>
-  </si>
-  <si>
-    <t>${detail.FISC_YEAR}</t>
-  </si>
-  <si>
-    <t>${detail.BUS_AREA}</t>
-  </si>
-  <si>
-    <t>${detail.DOC_DATE}</t>
-  </si>
-  <si>
-    <t>${detail.POST_DATE}</t>
-  </si>
-  <si>
-    <t>${detail.ENTRY_DATE}</t>
-  </si>
-  <si>
-    <t>${detail.DOC_HDR_TXT}</t>
-  </si>
-  <si>
-    <t>${detail.CURRENCY}</t>
-  </si>
-  <si>
-    <t>${detail.EXCH_RATE}</t>
-  </si>
-  <si>
-    <t>${detail.TRANS_TYPE}</t>
-  </si>
-  <si>
-    <t>${detail.OSS_ID}</t>
-  </si>
-  <si>
-    <t>${detail.SUMBER_DANA}</t>
-  </si>
-  <si>
-    <t>${detail.TGL_RENCANA_BYR}</t>
-  </si>
-  <si>
-    <t>${detail.BANK_BYR}</t>
-  </si>
-  <si>
-    <t>${detail.CURR_BAYAR}</t>
-  </si>
-  <si>
-    <t>${detail.BANK_BENEF}</t>
-  </si>
-  <si>
-    <t>${detail.NAMA_BENEF}</t>
-  </si>
-  <si>
-    <t>${detail.JENIS_BAYAR}</t>
-  </si>
-  <si>
-    <t>${detail.JENIS_DOC}</t>
-  </si>
-  <si>
-    <t>${detail.NAMA_UNIT}</t>
-  </si>
-  <si>
-    <t>${detail.TGL_TERIMA_INVOICE}</t>
-  </si>
-  <si>
-    <t>${detail.INPUT_BY}</t>
-  </si>
-  <si>
-    <t>${detail.LINE_NO}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_LC}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_TC}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_WITH_BASE_LC}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_WITH_LC}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_WITH_BASE_TC}</t>
-  </si>
-  <si>
-    <t>${detail.AMT_WITH_TC}</t>
-  </si>
-  <si>
-    <t>${detail.TOTAL_AMT_TC}</t>
-  </si>
-  <si>
-    <t>${detail.TOTAL_AMT_LC}</t>
-  </si>
-  <si>
-    <t>${detail.ASSIGNMENT}</t>
-  </si>
-  <si>
-    <t>${detail.ITEM_TEXT}</t>
-  </si>
-  <si>
-    <t>${detail.CUSTOMER}</t>
-  </si>
-  <si>
-    <t>${detail.CUSTOMER_NAME}</t>
-  </si>
-  <si>
-    <t>${detail.VENDOR_NAME}</t>
+    <t>JENIS TRANSAKSI</t>
+  </si>
+  <si>
+    <t>TIPE TRANSAKSI</t>
+  </si>
+  <si>
+    <t>AMOUNT BAYAR</t>
+  </si>
+  <si>
+    <t>EQ IDR</t>
+  </si>
+  <si>
+    <t>NAMA HOUSE BANK</t>
+  </si>
+  <si>
+    <t>CASH CODE</t>
+  </si>
+  <si>
+    <t>NAMA CASH CODE</t>
+  </si>
+  <si>
+    <t>TGL ENTRY</t>
+  </si>
+  <si>
+    <t>SUMBER DATA</t>
+  </si>
+  <si>
+    <t>${detail.JENIS_TRANSAKSI}</t>
+  </si>
+  <si>
+    <t>${detail.TIPE_TRANSAKSI}</t>
+  </si>
+  <si>
+    <t>${detail.CURRENCY_BAYAR}</t>
+  </si>
+  <si>
+    <t>${detail.EXCHANGE_RATE}</t>
+  </si>
+  <si>
+    <t>${detail.AMOUNT_BAYAR}</t>
+  </si>
+  <si>
+    <t>${detail.EQ_IDR}</t>
+  </si>
+  <si>
+    <t>${detail.HOUSE_BANK}</t>
+  </si>
+  <si>
+    <t>${detail.NAMA_HOUSE_BANK}</t>
+  </si>
+  <si>
+    <t>${detail.CASH_CODE}</t>
+  </si>
+  <si>
+    <t>${detail.NAMA_CASHCODE}</t>
+  </si>
+  <si>
+    <t>${detail.TGL_RENCANA_BAYAR}</t>
+  </si>
+  <si>
+    <t>${detail.TGL_ENTRY}</t>
+  </si>
+  <si>
+    <t>${detail.SUMBER_DATA}</t>
   </si>
 </sst>
 </file>
@@ -785,9 +635,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -828,6 +675,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1247,230 +1097,230 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA2A5E4-09F5-4CB0-B473-5EA81C63316C}">
   <dimension ref="A1:CE50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="4.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="19.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="27.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="34.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="27.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="24.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="22.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="26.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="24.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="63" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="65" width="15.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="28.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="28.875" style="2" customWidth="1"/>
-    <col min="68" max="68" width="27.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="17.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="30.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="25.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="23.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="21.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="20.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="22.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="21.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="21.75" style="2" customWidth="1"/>
-    <col min="82" max="82" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="24.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="11" style="2"/>
+    <col min="1" max="1" width="4.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="27.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="63" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="28.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.875" style="1" customWidth="1"/>
+    <col min="68" max="68" width="27.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="30.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="25.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="23.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="21.75" style="1" customWidth="1"/>
+    <col min="82" max="82" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" ht="18.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="17"/>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-      <c r="BB1" s="17"/>
-      <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
-      <c r="CB1" s="17"/>
-      <c r="CC1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+      <c r="AR1" s="18"/>
+      <c r="AS1" s="18"/>
+      <c r="AT1" s="18"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="18"/>
+      <c r="AW1" s="18"/>
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="16"/>
+      <c r="BD1" s="16"/>
+      <c r="BE1" s="16"/>
+      <c r="BF1" s="16"/>
+      <c r="BG1" s="16"/>
+      <c r="BH1" s="16"/>
+      <c r="BI1" s="16"/>
+      <c r="BJ1" s="16"/>
+      <c r="BK1" s="16"/>
+      <c r="BL1" s="16"/>
+      <c r="BM1" s="16"/>
+      <c r="BN1" s="16"/>
+      <c r="BO1" s="16"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="16"/>
+      <c r="BR1" s="16"/>
+      <c r="BS1" s="16"/>
+      <c r="BT1" s="16"/>
+      <c r="BU1" s="16"/>
+      <c r="BV1" s="16"/>
+      <c r="BW1" s="16"/>
+      <c r="BX1" s="16"/>
+      <c r="BY1" s="16"/>
+      <c r="BZ1" s="16"/>
+      <c r="CA1" s="16"/>
+      <c r="CB1" s="16"/>
+      <c r="CC1" s="16"/>
     </row>
     <row r="2" spans="1:83">
-      <c r="A2" s="11"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
     </row>
     <row r="3" spans="1:83">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1482,339 +1332,239 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
         <v>20</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+      <c r="AW3" s="7"/>
+    </row>
+    <row r="4" spans="1:83">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="AX4" s="9"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="9"/>
+      <c r="BC4" s="9"/>
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="9"/>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="9"/>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="9"/>
+      <c r="BO4" s="9"/>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="9"/>
+      <c r="BS4" s="9"/>
+      <c r="BT4" s="9"/>
+      <c r="BU4" s="9"/>
+      <c r="BV4" s="9"/>
+      <c r="BW4" s="9"/>
+      <c r="BX4" s="9"/>
+      <c r="BY4" s="9"/>
+      <c r="BZ4" s="9"/>
+      <c r="CA4" s="9"/>
+      <c r="CB4" s="9"/>
+      <c r="CC4" s="9"/>
+      <c r="CD4" s="7"/>
+      <c r="CE4" s="7"/>
+    </row>
+    <row r="5" spans="1:83">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:83" ht="31.5">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="P3" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="D6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="R3" t="s">
+      <c r="E6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="S3" t="s">
+      <c r="F6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T3" t="s">
+      <c r="G6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="U3" t="s">
+      <c r="H6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V3" t="s">
+      <c r="J6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W3" t="s">
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X3" t="s">
+      <c r="L6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="M6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="N6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="O6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO3"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-    </row>
-    <row r="4" spans="1:83">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="10"/>
-      <c r="BA4" s="10"/>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="10"/>
-      <c r="BE4" s="10"/>
-      <c r="BF4" s="10"/>
-      <c r="BG4" s="10"/>
-      <c r="BH4" s="10"/>
-      <c r="BI4" s="10"/>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="10"/>
-      <c r="BL4" s="10"/>
-      <c r="BM4" s="10"/>
-      <c r="BN4" s="10"/>
-      <c r="BO4" s="10"/>
-      <c r="BP4" s="10"/>
-      <c r="BQ4" s="10"/>
-      <c r="BR4" s="10"/>
-      <c r="BS4" s="10"/>
-      <c r="BT4" s="10"/>
-      <c r="BU4" s="10"/>
-      <c r="BV4" s="10"/>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="10"/>
-      <c r="BY4" s="10"/>
-      <c r="BZ4" s="10"/>
-      <c r="CA4" s="10"/>
-      <c r="CB4" s="10"/>
-      <c r="CC4" s="10"/>
-      <c r="CD4" s="8"/>
-      <c r="CE4" s="8"/>
-    </row>
-    <row r="5" spans="1:83">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:83" ht="31.5">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q6" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="U6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="V6" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="W6" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="X6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y6" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB6" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC6" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD6" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE6" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH6" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI6" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ6" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL6" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN6" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="18"/>
-      <c r="AR6" s="16"/>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="16"/>
-      <c r="AU6" s="16"/>
-      <c r="AV6" s="16"/>
-      <c r="AW6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="15"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
     </row>
     <row r="7" spans="1:83" ht="30.75">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="AX7" s="16"/>
-      <c r="AY7" s="16"/>
-      <c r="AZ7" s="16"/>
-      <c r="BA7" s="16"/>
-      <c r="BB7" s="16"/>
-      <c r="BC7" s="16"/>
-      <c r="BD7" s="16"/>
-      <c r="BE7" s="16"/>
-      <c r="BF7" s="16"/>
-      <c r="BG7" s="16"/>
-      <c r="BH7" s="16"/>
-      <c r="BI7" s="16"/>
-      <c r="BJ7" s="16"/>
-      <c r="BK7" s="16"/>
-      <c r="BL7" s="16"/>
-      <c r="BM7" s="16"/>
-      <c r="BN7" s="16"/>
-      <c r="BO7" s="16"/>
-      <c r="BP7" s="16"/>
-      <c r="BQ7" s="16"/>
-      <c r="BR7" s="8"/>
-      <c r="BU7" s="12"/>
-      <c r="BV7" s="12"/>
-      <c r="BW7" s="8"/>
-      <c r="CD7" s="8"/>
-      <c r="CE7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="AX7" s="15"/>
+      <c r="AY7" s="15"/>
+      <c r="AZ7" s="15"/>
+      <c r="BA7" s="15"/>
+      <c r="BB7" s="15"/>
+      <c r="BC7" s="15"/>
+      <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
+      <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="15"/>
+      <c r="BI7" s="15"/>
+      <c r="BJ7" s="15"/>
+      <c r="BK7" s="15"/>
+      <c r="BL7" s="15"/>
+      <c r="BM7" s="15"/>
+      <c r="BN7" s="15"/>
+      <c r="BO7" s="15"/>
+      <c r="BP7" s="15"/>
+      <c r="BQ7" s="15"/>
+      <c r="BR7" s="7"/>
+      <c r="BU7" s="11"/>
+      <c r="BV7" s="11"/>
+      <c r="BW7" s="7"/>
+      <c r="CD7" s="7"/>
+      <c r="CE7" s="7"/>
     </row>
     <row r="8" spans="1:83" ht="21">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:83">
-      <c r="AE9" s="7"/>
+      <c r="AE9" s="6"/>
     </row>
     <row r="10" spans="1:83">
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="9"/>
-      <c r="AH10" s="9"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="8"/>
+      <c r="AH10" s="8"/>
     </row>
     <row r="11" spans="1:83">
       <c r="D11"/>
+      <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:83">
       <c r="D12"/>

</xml_diff>